<commit_message>
Servo-Rail assembly and Case
</commit_message>
<xml_diff>
--- a/documentation/Protocol.xlsx
+++ b/documentation/Protocol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Just Data\Projects\Servostation\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Just data\Projects\Servostation\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70BDE09-C641-4C1D-98BB-BFD19A579229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79546338-88DC-4C53-A297-2F6201299FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workhours" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Work Hours</t>
   </si>
@@ -72,19 +72,47 @@
   </si>
   <si>
     <t>Continued on software</t>
+  </si>
+  <si>
+    <t>Designed input and output panels</t>
+  </si>
+  <si>
+    <t>Constructed servo mounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constructed basic case </t>
+  </si>
+  <si>
+    <t>Constructed servo-rail assembly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -112,17 +140,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,126 +571,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" customWidth="1"/>
     <col min="4" max="4" width="60.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="1">
+      <c r="B4" s="9">
         <v>44936</v>
       </c>
       <c r="C4" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="1">
+      <c r="B5" s="9">
         <v>44940</v>
       </c>
       <c r="C5" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="1">
+      <c r="B6" s="9">
         <v>44943</v>
       </c>
       <c r="C6" s="2">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="1">
+      <c r="B7" s="9">
         <v>44943</v>
       </c>
       <c r="C7" s="2">
         <v>0.125</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
+      <c r="B8" s="9">
         <v>44943</v>
       </c>
       <c r="C8" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="1">
+      <c r="B9" s="9">
         <v>44944</v>
       </c>
       <c r="C9" s="2">
         <v>0.25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="1">
+      <c r="B10" s="9">
         <v>44944</v>
       </c>
       <c r="C10" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="9">
+        <v>44945</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+      <c r="B12" s="9">
+        <v>44945</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="9">
+        <v>44945</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="9">
+        <v>44945</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="10"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2">
-        <f>SUM(C4:C11)</f>
-        <v>0.75000000000000011</v>
-      </c>
-    </row>
+      <c r="C16" s="12">
+        <f>SUM(C4:C15)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
software and electronics update
</commit_message>
<xml_diff>
--- a/documentation/Protocol.xlsx
+++ b/documentation/Protocol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Just data\Projects\Servostation\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Just Data\Projects\Servostation\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01FDB06-3C59-446E-AEA0-C9BFEF286C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B49C9E-39B6-4CCA-A75D-579D64EAA4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workhours" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Work Hours</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Writing documentation</t>
+  </si>
+  <si>
+    <t>Drawing sketches</t>
+  </si>
+  <si>
+    <t>Designing electronics and printing first test parts</t>
   </si>
 </sst>
 </file>
@@ -574,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,21 +744,59 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="10"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="11" t="s">
+      <c r="B16" s="9">
+        <v>44947</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="9">
+        <v>44948</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="9">
+        <v>44949</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="9"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="10"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="12">
-        <f>SUM(C4:C16)</f>
-        <v>1.041666666666667</v>
-      </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="C21" s="12">
+        <f>SUM(C4:C20)</f>
+        <v>1.2916666666666672</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>